<commit_message>
Check list Krotov Home Work test mobil game
</commit_message>
<xml_diff>
--- a/Чек-лист-Кротов-webдодаток(UK).xlsx
+++ b/Чек-лист-Кротов-webдодаток(UK).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="161">
   <si>
     <t>Браузер версія</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Passed</t>
-  </si>
-  <si>
-    <t>Версія ОС</t>
   </si>
   <si>
     <t>Відображення елементів сторінок</t>
@@ -290,12 +287,6 @@
     <t>Перевірити коректне відображення спливаючих вікон з помилками/повідомленнями</t>
   </si>
   <si>
-    <t>Назва додатку</t>
-  </si>
-  <si>
-    <t>Назва та модель моб. пристрою</t>
-  </si>
-  <si>
     <t>Функції на пристроях</t>
   </si>
   <si>
@@ -493,6 +484,33 @@
   </si>
   <si>
     <t>Для дзвінка до Франції потрібно використовувати наступний формат номерів: «+33-хх-хх-хх-хх-хх» локалізацію номерів телефонів не пройдено</t>
+  </si>
+  <si>
+    <t>Wallken Runner</t>
+  </si>
+  <si>
+    <t>Гра продовжується при вхідному дзвінку , а при натисканні відповіді гра закривається з втрачанням енергії ресурсів і т. п.</t>
+  </si>
+  <si>
+    <t>Відсутність крешей при проходженні гри</t>
+  </si>
+  <si>
+    <t>Перевірити чи працює функція підвищення рівня</t>
+  </si>
+  <si>
+    <t>Превірити чи з підвищенням рівня підвищуються характеристики ігрового персонажу</t>
+  </si>
+  <si>
+    <t>Після перегляду реклами можливий креш з втратою бонусу за перегляд реклами і виходом з гри</t>
+  </si>
+  <si>
+    <t>Підвищення характеристик Attack і Health завмерли на рівні 139 і 179 відповідно.</t>
+  </si>
+  <si>
+    <t>Перевірити механіку "point and tap "</t>
+  </si>
+  <si>
+    <t>Перевірити механіку "drag and drop"</t>
   </si>
 </sst>
 </file>
@@ -795,6 +813,15 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -804,21 +831,12 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="96">
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -935,6 +953,798 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF00FF00"/>
           <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFEFEF"/>
+          <bgColor rgb="FFEFEFEF"/>
         </patternFill>
       </fill>
       <alignment wrapText="1" shrinkToFit="0"/>
@@ -2023,7 +2833,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2052,22 +2862,22 @@
   <sheetData>
     <row r="1" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -2084,31 +2894,31 @@
     </row>
     <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:18" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>123</v>
-      </c>
       <c r="B3" s="29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C3" s="39" t="s">
         <v>6</v>
@@ -2120,44 +2930,44 @@
         <v>6</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>4</v>
@@ -2169,37 +2979,37 @@
         <v>4</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G5" s="38" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>6</v>
@@ -2214,36 +3024,36 @@
     </row>
     <row r="8" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G9" s="6"/>
     </row>
@@ -2251,13 +3061,13 @@
       <c r="A10" s="6"/>
       <c r="B10" s="29"/>
       <c r="C10" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -2265,13 +3075,13 @@
     <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="C11" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="6"/>
@@ -2279,13 +3089,13 @@
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="C12" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -2293,13 +3103,13 @@
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="C13" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -2308,13 +3118,13 @@
       <c r="A14" s="40"/>
       <c r="B14" s="29"/>
       <c r="C14" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -2323,13 +3133,13 @@
       <c r="A15" s="40"/>
       <c r="B15" s="29"/>
       <c r="C15" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -2369,7 +3179,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -2383,22 +3193,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G3:G5 C22:E23 C1:E15">
-    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5 C22:E23 C1:E15">
-    <cfRule type="containsText" dxfId="50" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5 C22:E23 C1:E15">
-    <cfRule type="containsText" dxfId="49" priority="3" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5 C22:E23 C1:E15">
-    <cfRule type="containsText" dxfId="48" priority="4" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2432,7 +3242,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="32" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>0</v>
@@ -2444,7 +3254,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
@@ -2460,12 +3270,12 @@
       <c r="Q1" s="31"/>
     </row>
     <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
@@ -2495,10 +3305,10 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -2513,25 +3323,25 @@
     </row>
     <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -2546,23 +3356,23 @@
     </row>
     <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -2577,16 +3387,16 @@
     </row>
     <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -2603,12 +3413,12 @@
       <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
-        <v>26</v>
+      <c r="A7" s="45" t="s">
+        <v>25</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2625,16 +3435,16 @@
     </row>
     <row r="8" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2652,16 +3462,16 @@
     </row>
     <row r="9" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2679,16 +3489,16 @@
     </row>
     <row r="10" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -2706,16 +3516,16 @@
     </row>
     <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -2732,12 +3542,12 @@
       <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
-        <v>41</v>
+      <c r="A12" s="45" t="s">
+        <v>40</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
@@ -2754,16 +3564,16 @@
     </row>
     <row r="13" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -2781,16 +3591,16 @@
     </row>
     <row r="14" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -2807,12 +3617,12 @@
       <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
-        <v>45</v>
+      <c r="A15" s="45" t="s">
+        <v>44</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
@@ -2829,16 +3639,16 @@
     </row>
     <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -2875,7 +3685,7 @@
     </row>
     <row r="18" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -2956,7 +3766,7 @@
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -21562,22 +22372,22 @@
     <mergeCell ref="A15:D15"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:D1 B3:D4 F3:F5 B26:D1000 B17:D24 B5">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="91" priority="1" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1 B3:D4 F3:F5 B26:D1000 B17:D24 B5">
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="90" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1 B3:D4 F3:F5 B26:D1000 B17:D24 B5">
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="89" priority="3" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1 B3:D4 F3:F5 B26:D1000 B17:D24 B5">
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="88" priority="4" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21611,22 +22421,22 @@
   <sheetData>
     <row r="1" spans="1:18" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -21643,58 +22453,58 @@
     </row>
     <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
       <c r="C2" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B4" s="29" t="s">
         <v>80</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>81</v>
       </c>
       <c r="C4" s="39" t="s">
         <v>6</v>
@@ -21709,15 +22519,15 @@
         <v>6</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>6</v>
@@ -21733,15 +22543,15 @@
         <v>4</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="39" t="s">
         <v>6</v>
@@ -21758,10 +22568,10 @@
     </row>
     <row r="7" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>6</v>
@@ -21778,10 +22588,10 @@
     </row>
     <row r="8" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>6</v>
@@ -21798,32 +22608,32 @@
     </row>
     <row r="9" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>76</v>
-      </c>
       <c r="C9" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C10" s="39" t="s">
         <v>6</v>
@@ -21840,22 +22650,22 @@
     </row>
     <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
         <v>78</v>
       </c>
-      <c r="B11" t="s">
-        <v>79</v>
-      </c>
       <c r="C11" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="20"/>
@@ -21871,7 +22681,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -21882,10 +22692,10 @@
     </row>
     <row r="14" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C14" s="39" t="s">
         <v>6</v>
@@ -21902,10 +22712,10 @@
     </row>
     <row r="15" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C15" s="39" t="s">
         <v>6</v>
@@ -21984,7 +22794,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -22000,22 +22810,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G3:G5 C1:E11 C14:E15 C22:E23">
-    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="87" priority="1" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5 C1:E11 C14:E15 C22:E23">
-    <cfRule type="containsText" dxfId="42" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="86" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5 C1:E11 C14:E15 C22:E23">
-    <cfRule type="containsText" dxfId="41" priority="3" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="85" priority="3" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5 C1:E11 C14:E15 C22:E23">
-    <cfRule type="containsText" dxfId="40" priority="4" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="84" priority="4" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22054,7 +22864,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>0</v>
@@ -22066,7 +22876,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -22115,15 +22925,15 @@
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
@@ -22138,26 +22948,26 @@
     </row>
     <row r="4" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -22172,7 +22982,7 @@
     </row>
     <row r="5" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -22183,7 +22993,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -22198,16 +23008,16 @@
     </row>
     <row r="6" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -22226,16 +23036,16 @@
     </row>
     <row r="7" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -22254,16 +23064,16 @@
     </row>
     <row r="8" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -22282,7 +23092,7 @@
     </row>
     <row r="9" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -22304,16 +23114,16 @@
     </row>
     <row r="10" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -22332,16 +23142,16 @@
     </row>
     <row r="11" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -22360,16 +23170,16 @@
     </row>
     <row r="12" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -22388,16 +23198,16 @@
     </row>
     <row r="13" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -22416,16 +23226,16 @@
     </row>
     <row r="14" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -22444,16 +23254,16 @@
     </row>
     <row r="15" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -22472,7 +23282,7 @@
     </row>
     <row r="16" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -22494,16 +23304,16 @@
     </row>
     <row r="17" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -22522,16 +23332,16 @@
     </row>
     <row r="18" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -22550,16 +23360,16 @@
     </row>
     <row r="19" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -22578,16 +23388,16 @@
     </row>
     <row r="20" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -22606,16 +23416,16 @@
     </row>
     <row r="21" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -22634,7 +23444,7 @@
     </row>
     <row r="22" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -22656,16 +23466,16 @@
     </row>
     <row r="23" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -22684,16 +23494,16 @@
     </row>
     <row r="24" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -22712,16 +23522,16 @@
     </row>
     <row r="25" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -22740,16 +23550,16 @@
     </row>
     <row r="26" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -22788,7 +23598,7 @@
     </row>
     <row r="28" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -42250,62 +43060,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:D1 G3:G5 C3 F1:H1">
-    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36 B37:H37 B27:H35 E7:H26">
-    <cfRule type="containsText" dxfId="38" priority="2" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(B7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1 G3:G5 C3 F1:H1">
-    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36 B37:H37 B27:H35 E7:H26">
-    <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(B7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1 G3:G5 C3 F1:H1">
-    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36 B37:H37 B27:H35 E7:H26">
-    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(B7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1 G3:G5 C3 F1:H1">
-    <cfRule type="containsText" dxfId="33" priority="7" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="77" priority="7" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:H36 B37:H37 B27:H35 E7:H26">
-    <cfRule type="containsText" dxfId="32" priority="8" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="76" priority="8" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(B7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5">
-    <cfRule type="containsText" dxfId="31" priority="9" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5">
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5">
-    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G5">
-    <cfRule type="containsText" dxfId="28" priority="12" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42323,9 +43133,9 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -42341,14 +43151,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
-        <v>137</v>
+      <c r="A1" s="43" t="s">
+        <v>134</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -42365,9 +43175,9 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
+      <c r="A2" s="42"/>
       <c r="B2" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -42387,7 +43197,7 @@
     <row r="3" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -42406,16 +43216,16 @@
     </row>
     <row r="4" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="44" t="s">
-        <v>10</v>
+      <c r="E4" s="47" t="s">
+        <v>9</v>
       </c>
-      <c r="F4" s="43" t="s">
-        <v>84</v>
+      <c r="F4" s="46" t="s">
+        <v>83</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -42430,15 +43240,15 @@
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="43"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -42452,20 +43262,20 @@
     </row>
     <row r="6" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -42480,7 +43290,7 @@
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>6</v>
@@ -42491,7 +43301,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -42506,13 +43316,13 @@
     </row>
     <row r="8" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -42530,10 +43340,10 @@
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -42552,7 +43362,7 @@
     </row>
     <row r="10" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>6</v>
@@ -42574,7 +43384,7 @@
     </row>
     <row r="11" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>6</v>
@@ -42596,7 +43406,7 @@
     </row>
     <row r="12" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>6</v>
@@ -42618,7 +43428,7 @@
     </row>
     <row r="13" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>6</v>
@@ -42640,13 +43450,13 @@
     </row>
     <row r="14" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -42664,13 +43474,13 @@
     </row>
     <row r="15" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -42688,13 +43498,13 @@
     </row>
     <row r="16" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -42712,7 +43522,7 @@
     </row>
     <row r="17" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>6</v>
@@ -42734,13 +43544,13 @@
     </row>
     <row r="18" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -42758,7 +43568,7 @@
     </row>
     <row r="19" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>6</v>
@@ -42798,7 +43608,7 @@
     </row>
     <row r="21" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>6</v>
@@ -42820,13 +43630,13 @@
     </row>
     <row r="22" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -42844,13 +43654,13 @@
     </row>
     <row r="23" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -42868,7 +43678,7 @@
     </row>
     <row r="24" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>6</v>
@@ -42890,7 +43700,7 @@
     </row>
     <row r="25" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>6</v>
@@ -42912,7 +43722,7 @@
     </row>
     <row r="26" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>6</v>
@@ -42934,7 +43744,7 @@
     </row>
     <row r="27" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="40" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>6</v>
@@ -42956,13 +43766,13 @@
     </row>
     <row r="28" spans="1:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
-      <c r="B28" s="47" t="s">
-        <v>10</v>
+      <c r="B28" s="44" t="s">
+        <v>9</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -60480,42 +61290,42 @@
     <mergeCell ref="E4:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B3 C2:D5 E1:F3 G1:J1000 F8:F1000 B30:B1000 D30:D1000 C49:C1000 C7:D28 D6 D1 E6:E1000 E4 B5:B28">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3 C2:D5 E1:F3 G1:J1000 F8:F1000 B30:B1000 D30:D1000 C49:C1000 C7:D28 D6 D1 E6:E1000 E4 B5:B28">
-    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="70" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3 C2:D5 E1:F3 G1:J1000 F8:F1000 B30:B1000 D30:D1000 C49:C1000 C7:D28 D6 D1 E6:E1000 E4 B5:B28">
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3 C2:D5 E1:F3 G1:J1000 F8:F1000 B30:B1000 D30:D1000 C49:C1000 C7:D28 D6 D1 E6:E1000 E4 B5:B28">
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="65" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="containsText" dxfId="20" priority="8" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="64" priority="8" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -60532,8 +61342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -60544,15 +61354,15 @@
     <col min="6" max="6" width="89.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -60561,7 +61371,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="8" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -60570,51 +61380,51 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="44" t="s">
-        <v>10</v>
+      <c r="E3" s="47" t="s">
+        <v>9</v>
       </c>
-      <c r="F3" s="43" t="s">
-        <v>84</v>
+      <c r="F3" s="46" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="43"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>4</v>
@@ -60625,12 +61435,12 @@
         <v>4</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -60640,22 +61450,22 @@
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
+      <c r="B8" s="22" t="s">
+        <v>4</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
+      <c r="B9" s="22" t="s">
+        <v>4</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -60664,7 +61474,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -60672,24 +61482,24 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>11</v>
+      <c r="B11" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>11</v>
+      <c r="B12" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -60698,7 +61508,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -60706,48 +61516,50 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>11</v>
+      <c r="B14" s="22" t="s">
+        <v>6</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>11</v>
+      <c r="B15" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>11</v>
+      <c r="B16" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>11</v>
+      <c r="B17" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -60756,7 +61568,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -60764,12 +61576,12 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>11</v>
+      <c r="B19" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -60778,40 +61590,85 @@
     </row>
     <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>11</v>
+      <c r="B20" s="22" t="s">
+        <v>6</v>
       </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="20"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+    </row>
+    <row r="23" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
+      <c r="B30" s="22" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="6"/>
@@ -60846,44 +61703,64 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B2 E1:F2 B4:B6 D5 D1 E3 C2:D4 F7:F19 C6:D19 E5:E19 B34:F37">
-    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="not run">
+  <conditionalFormatting sqref="B2 E1:F2 D5 D1 E3 C2:D4 F7:F19 C6:D19 E5:E19 B34:F37 B4:B20 B23:B30">
+    <cfRule type="containsText" dxfId="63" priority="5" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2 E1:F2 B4:B6 D5 D1 E3 C2:D4 F7:F19 C6:D19 E5:E19 B34:F37">
-    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="Passed">
+  <conditionalFormatting sqref="B2 E1:F2 D5 D1 E3 C2:D4 F7:F19 C6:D19 E5:E19 B34:F37 B4:B20 B23:B30">
+    <cfRule type="containsText" dxfId="62" priority="6" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2 E1:F2 B4:B6 D5 D1 E3 C2:D4 F7:F19 C6:D19 E5:E19 B34:F37">
-    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="B2 E1:F2 D5 D1 E3 C2:D4 F7:F19 C6:D19 E5:E19 B34:F37 B4:B20 B23:B30">
+    <cfRule type="containsText" dxfId="61" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2 E1:F2 B4:B6 D5 D1 E3 C2:D4 F7:F19 C6:D19 E5:E19 B34:F37">
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Skipped">
+  <conditionalFormatting sqref="B2 E1:F2 D5 D1 E3 C2:D4 F7:F19 C6:D19 E5:E19 B34:F37 B4:B20 B23:B30">
+    <cfRule type="containsText" dxfId="60" priority="8" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="not run">
+    <cfRule type="containsText" dxfId="59" priority="9" operator="containsText" text="not run">
       <formula>NOT(ISERROR(SEARCH(("not run"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="58" priority="10" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH(("Passed"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="57" priority="11" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(A2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="Skipped">
+    <cfRule type="containsText" dxfId="56" priority="12" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(A2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="not run">
+      <formula>NOT(ISERROR(SEARCH(("not run"),(B1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH(("Passed"),(B1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH(("Failed"),(B1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="containsText" dxfId="45" priority="4" operator="containsText" text="Skipped">
+      <formula>NOT(ISERROR(SEARCH(("Skipped"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>